<commit_message>
First 4 ES video sequences
</commit_message>
<xml_diff>
--- a/data/Dataset_preprocessing.xlsx
+++ b/data/Dataset_preprocessing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basil\Documents\Work\UQAC\S2\Séminaire\SeminaireIA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F169282-BAAE-45B7-9D8F-B340ED5D4F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5DBE59-159F-4655-A606-40AAE018EE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E80DD2AD-FA2C-43F2-848E-4CD4E87C2301}"/>
   </bookViews>
@@ -766,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{503B799C-B42A-47E4-858C-2ED052BB6473}">
-  <dimension ref="A1:CG22"/>
+  <dimension ref="A1:CG23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1529,53 +1529,600 @@
       <c r="B16" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f>COUNT(D16:CY16)</f>
+        <v>38</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4.7222222222222221E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="G16" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.10138888888888889</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.11944444444444445</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.15138888888888888</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.17222222222222222</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="O16" s="2">
+        <v>0.23680555555555555</v>
+      </c>
+      <c r="P16" s="2">
+        <v>0.24444444444444444</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="R16" s="2">
+        <v>0.27708333333333335</v>
+      </c>
+      <c r="S16" s="2">
+        <v>0.28680555555555554</v>
+      </c>
+      <c r="T16" s="2">
+        <v>0.29444444444444445</v>
+      </c>
+      <c r="U16" s="2">
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="V16" s="2">
+        <v>0.31319444444444444</v>
+      </c>
+      <c r="W16" s="2">
+        <v>0.32013888888888886</v>
+      </c>
+      <c r="X16" s="2">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="Y16" s="2">
+        <v>0.35208333333333336</v>
+      </c>
+      <c r="Z16" s="2">
+        <v>0.36527777777777776</v>
+      </c>
+      <c r="AA16" s="2">
+        <v>0.37291666666666667</v>
+      </c>
+      <c r="AB16" s="2">
+        <v>0.40208333333333335</v>
+      </c>
+      <c r="AC16" s="2">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="AD16" s="2">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="AE16" s="2">
+        <v>0.43402777777777779</v>
+      </c>
+      <c r="AF16" s="2">
+        <v>0.46041666666666664</v>
+      </c>
+      <c r="AG16" s="2">
+        <v>0.46805555555555556</v>
+      </c>
+      <c r="AH16" s="2">
+        <v>0.47638888888888886</v>
+      </c>
+      <c r="AI16" s="2">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="AJ16" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="AK16" s="2">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="AL16" s="2">
+        <v>0.53680555555555554</v>
+      </c>
+      <c r="AM16" s="2">
+        <v>0.5444444444444444</v>
+      </c>
+      <c r="AN16" s="2">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="AO16" s="2">
+        <v>0.58611111111111114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <f t="shared" ref="C17:C22" si="0">COUNT(D17:CY17)</f>
+        <v>15</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5.8333333333333334E-2</v>
+      </c>
+      <c r="E17" s="2">
+        <v>6.805555555555555E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.11458333333333333</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.17291666666666666</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.2048611111111111</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.21180555555555555</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.25972222222222224</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.27430555555555558</v>
+      </c>
+      <c r="N17" s="2">
+        <v>0.33055555555555555</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="P17" s="2">
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="R17" s="2">
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2.5694444444444443E-2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="I18" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="J18" s="2">
+        <v>6.0416666666666667E-2</v>
+      </c>
+      <c r="K18" s="2">
+        <v>7.0833333333333331E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>8.5416666666666669E-2</v>
+      </c>
+      <c r="M18" s="2">
+        <v>9.4444444444444442E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <v>0.10486111111111111</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0.12916666666666668</v>
+      </c>
+      <c r="P18" s="2">
+        <v>0.14097222222222222</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>0.14861111111111111</v>
+      </c>
+      <c r="R18" s="2">
+        <v>0.17291666666666666</v>
+      </c>
+      <c r="S18" s="2">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="T18" s="2">
+        <v>0.18888888888888888</v>
+      </c>
+      <c r="U18" s="2">
+        <v>0.20902777777777778</v>
+      </c>
+      <c r="V18" s="2">
+        <v>0.21666666666666667</v>
+      </c>
+      <c r="W18" s="2">
+        <v>0.22638888888888889</v>
+      </c>
+      <c r="X18" s="2">
+        <v>0.23402777777777778</v>
+      </c>
+      <c r="Y18" s="2">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>0.27847222222222223</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>0.30972222222222223</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>0.31736111111111109</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>0.32847222222222222</v>
+      </c>
+      <c r="AG18" s="2">
+        <v>0.33611111111111114</v>
+      </c>
+      <c r="AH18" s="2">
+        <v>0.35208333333333336</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="AJ18" s="2">
+        <v>0.41875000000000001</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>0.42638888888888887</v>
+      </c>
+      <c r="AL18" s="2">
+        <v>0.44027777777777777</v>
+      </c>
+      <c r="AM18" s="2">
+        <v>0.44722222222222224</v>
+      </c>
+      <c r="AN18" s="2">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="AO18" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="AP18" s="2">
+        <v>0.49027777777777776</v>
+      </c>
+      <c r="AQ18" s="2">
+        <v>0.49791666666666667</v>
+      </c>
+      <c r="AR18" s="2">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="AS18" s="2">
+        <v>0.51458333333333328</v>
+      </c>
+      <c r="AT18" s="2">
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="AU18" s="2">
+        <v>0.54722222222222228</v>
+      </c>
+      <c r="AV18" s="2">
+        <v>0.55486111111111114</v>
+      </c>
+      <c r="AW18" s="2">
+        <v>0.56874999999999998</v>
+      </c>
+      <c r="AX18" s="2">
+        <v>0.57638888888888884</v>
+      </c>
+      <c r="AY18" s="2">
+        <v>0.58402777777777781</v>
+      </c>
+      <c r="AZ18" s="2">
+        <v>0.59305555555555556</v>
+      </c>
+      <c r="BA18" s="2">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="BB18" s="2">
+        <v>0.62083333333333335</v>
+      </c>
+      <c r="BC18" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="BD18" s="2">
+        <v>0.64236111111111116</v>
+      </c>
+      <c r="BE18" s="2">
+        <v>0.64930555555555558</v>
+      </c>
+      <c r="BF18" s="2">
+        <v>0.65694444444444444</v>
+      </c>
+      <c r="BG18" s="2">
+        <v>0.6645833333333333</v>
+      </c>
+      <c r="BH18" s="2">
+        <v>0.67222222222222228</v>
+      </c>
+      <c r="BI18" s="2">
+        <v>0.68125000000000002</v>
+      </c>
+      <c r="BJ18" s="2">
+        <v>0.70416666666666672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <v>5.1388888888888887E-2</v>
+      </c>
+      <c r="I19" s="2">
+        <v>5.9027777777777776E-2</v>
+      </c>
+      <c r="J19" s="2">
+        <v>7.1527777777777773E-2</v>
+      </c>
+      <c r="K19" s="2">
+        <v>8.4027777777777785E-2</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.10277777777777777</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.11041666666666666</v>
+      </c>
+      <c r="N19" s="2">
+        <v>0.12291666666666666</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.13263888888888889</v>
+      </c>
+      <c r="P19" s="2">
+        <v>0.14027777777777778</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>0.14791666666666667</v>
+      </c>
+      <c r="R19" s="2">
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="S19" s="2">
+        <v>0.17291666666666666</v>
+      </c>
+      <c r="T19" s="2">
+        <v>0.18055555555555555</v>
+      </c>
+      <c r="U19" s="2">
+        <v>0.18819444444444444</v>
+      </c>
+      <c r="V19" s="2">
+        <v>0.19583333333333333</v>
+      </c>
+      <c r="W19" s="2">
+        <v>0.21527777777777779</v>
+      </c>
+      <c r="X19" s="2">
+        <v>0.23194444444444445</v>
+      </c>
+      <c r="Y19" s="2">
+        <v>0.23958333333333334</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>0.24722222222222223</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>0.25486111111111109</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>0.26250000000000001</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>0.27013888888888887</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>0.2902777777777778</v>
+      </c>
+      <c r="AF19" s="2">
+        <v>0.29791666666666666</v>
+      </c>
+      <c r="AG19" s="2">
+        <v>0.30555555555555558</v>
+      </c>
+      <c r="AH19" s="2">
+        <v>0.33263888888888887</v>
+      </c>
+      <c r="AI19" s="2">
+        <v>0.34027777777777779</v>
+      </c>
+      <c r="AJ19" s="2">
+        <v>0.34791666666666665</v>
+      </c>
+      <c r="AK19" s="2">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="AM19" s="2">
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="AN19" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="AO19" s="2">
+        <v>0.39305555555555555</v>
+      </c>
+      <c r="AP19" s="2">
+        <v>0.40069444444444446</v>
+      </c>
+      <c r="AQ19" s="2">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="AR19" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="AS19" s="2">
+        <v>0.43680555555555556</v>
+      </c>
+      <c r="AT19" s="2">
+        <v>0.44722222222222224</v>
+      </c>
+      <c r="AU19" s="2">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="AV19" s="2">
+        <v>0.46250000000000002</v>
+      </c>
+      <c r="AW19" s="2">
+        <v>0.47013888888888888</v>
+      </c>
+      <c r="AX19" s="2">
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="AY19" s="2">
+        <v>0.49444444444444446</v>
+      </c>
+      <c r="AZ19" s="2">
+        <v>0.50208333333333333</v>
+      </c>
+      <c r="BA19" s="2">
+        <v>0.50972222222222219</v>
+      </c>
+      <c r="BB19" s="2">
+        <v>0.51736111111111116</v>
+      </c>
+      <c r="BC19" s="2">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="BD19" s="2">
+        <v>0.54513888888888884</v>
+      </c>
+      <c r="BE19" s="2">
+        <v>0.55277777777777781</v>
+      </c>
+      <c r="BF19" s="2">
+        <v>0.56041666666666667</v>
+      </c>
+      <c r="BG19" s="2">
+        <v>0.58125000000000004</v>
+      </c>
+      <c r="BH19" s="2">
+        <v>0.59375</v>
+      </c>
+      <c r="BI19" s="2">
+        <v>0.6069444444444444</v>
+      </c>
+      <c r="BJ19" s="2">
+        <v>0.61597222222222225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:62" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>101</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:62" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <f>SUM(C16:C22)</f>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -1588,8 +2135,9 @@
     <hyperlink ref="B12" r:id="rId5" tooltip="https://www.youtube.com/watch?v=k6xCuRi9wUk" xr:uid="{BC5D6943-6684-4B51-B5D5-A9C58AAD6AFD}"/>
     <hyperlink ref="B8" r:id="rId6" xr:uid="{EEE00EC1-D55A-4149-837C-3F8E1983EF26}"/>
     <hyperlink ref="B9" r:id="rId7" xr:uid="{80D9DCE7-CFCF-434C-B3CB-7E3B789CD3CF}"/>
+    <hyperlink ref="B16" r:id="rId8" xr:uid="{9790B692-FC71-4B34-90D8-8A506DFAD353}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>